<commit_message>
added log on extent report
</commit_message>
<xml_diff>
--- a/reports/API_Report/api.xlsx
+++ b/reports/API_Report/api.xlsx
@@ -229,16 +229,16 @@
     <t>DEVICE NAME</t>
   </si>
   <si>
-    <t>Apr 25, 2025 8:15:16 am</t>
+    <t>Apr 26, 2025 9:17:48 pm</t>
   </si>
   <si>
-    <t>Apr 25, 2025 8:15:08 am</t>
+    <t>Apr 26, 2025 9:17:40 pm</t>
   </si>
   <si>
-    <t>Apr 25, 2025 8:15:14 am</t>
+    <t>Apr 26, 2025 9:17:46 pm</t>
   </si>
   <si>
-    <t>6.077 s</t>
+    <t>5.655 s</t>
   </si>
   <si>
     <t>0%</t>
@@ -268,16 +268,16 @@
     <t>Verify if Place is being Successfully added using AddPlaceAPI</t>
   </si>
   <si>
-    <t>2.137 s</t>
+    <t>2.016 s</t>
   </si>
   <si>
     <t>Verify if Place is being Successfully get using GetSinglePlaceAPI</t>
   </si>
   <si>
-    <t>1.328 s</t>
+    <t>1.280 s</t>
   </si>
   <si>
-    <t>1.962 s</t>
+    <t>1.799 s</t>
   </si>
   <si>
     <t>@AddPlace</t>
@@ -289,7 +289,7 @@
     <t>@GetPerson</t>
   </si>
   <si>
-    <t>5.442 s</t>
+    <t>5.111 s</t>
   </si>
   <si>
     <t>Then the "DeletePlaceAPI" Call got success with status code "400"</t>
@@ -301,7 +301,7 @@
 	at org.junit.Assert.assertEquals(Assert.java:128)
 	at org.junit.Assert.assertEquals(Assert.java:472)
 	at org.junit.Assert.assertEquals(Assert.java:456)
-	at stepDefinitions.StepDefinition.the_Call_got_success_with_status_code(StepDefinition.java:171)
+	at stepDefinitions.StepDefinition.the_Call_got_success_with_status_code(StepDefinition.java:156)
 	at ✽.the "DeletePlaceAPI" Call got success with status code "400"(file:///D:/eatOS/Appium/RahulShettyBDDAPIFramework/src/test/java/features/placeValidation.feature:34)
 </t>
   </si>
@@ -8695,7 +8695,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="EED3" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="C90D" scenarios="true" objects="true"/>
   <mergeCells count="10">
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="B63:C63"/>
@@ -9362,7 +9362,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="F78D" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="BD0F" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>